<commit_message>
Update docs Requirement architecture feedback
</commit_message>
<xml_diff>
--- a/docs/Planning en Urenverantwoording/Urenplanning en verantwoording.xlsx
+++ b/docs/Planning en Urenverantwoording/Urenplanning en verantwoording.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t>Themaopdracht 6</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>constraints model</t>
+  </si>
+  <si>
+    <t>MoSCoW</t>
+  </si>
+  <si>
+    <t>Use Case verbetering</t>
   </si>
   <si>
     <t>technisch verslag</t>
@@ -597,7 +603,9 @@
     <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -2290,7 +2298,9 @@
       <c r="G35" s="65">
         <v>1.5</v>
       </c>
-      <c r="H35" s="68"/>
+      <c r="H35" s="65">
+        <v>1.5</v>
+      </c>
       <c r="I35" s="26"/>
       <c r="J35" s="26"/>
       <c r="K35" s="69"/>
@@ -2301,7 +2311,7 @@
       </c>
       <c r="N35" s="26" t="str">
         <f t="shared" si="28"/>
-        <v>0.0</v>
+        <v>1.5</v>
       </c>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
@@ -2424,7 +2434,9 @@
       <c r="E38" s="64">
         <v>2.0</v>
       </c>
-      <c r="F38" s="64"/>
+      <c r="F38" s="64">
+        <v>2.0</v>
+      </c>
       <c r="G38" s="65"/>
       <c r="H38" s="65"/>
       <c r="I38" s="26"/>
@@ -2432,7 +2444,9 @@
       <c r="K38" s="66">
         <v>2.0</v>
       </c>
-      <c r="L38" s="66"/>
+      <c r="L38" s="66">
+        <v>2.0</v>
+      </c>
       <c r="M38" s="25"/>
       <c r="N38" s="26"/>
       <c r="O38" s="3"/>
@@ -2464,7 +2478,9 @@
       <c r="G39" s="65">
         <v>2.5</v>
       </c>
-      <c r="H39" s="65"/>
+      <c r="H39" s="65">
+        <v>2.5</v>
+      </c>
       <c r="I39" s="26"/>
       <c r="J39" s="26"/>
       <c r="K39" s="66"/>
@@ -2519,8 +2535,12 @@
       <c r="Z40" s="3"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="14"/>
-      <c r="B41" s="78"/>
+      <c r="A41" s="29">
+        <v>4.0</v>
+      </c>
+      <c r="B41" s="78" t="s">
+        <v>43</v>
+      </c>
       <c r="C41" s="67"/>
       <c r="D41" s="67"/>
       <c r="E41" s="26"/>
@@ -2547,12 +2567,8 @@
       <c r="Z41" s="3"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="14">
-        <v>5.0</v>
-      </c>
-      <c r="B42" s="56" t="s">
-        <v>43</v>
-      </c>
+      <c r="A42" s="29"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="67"/>
       <c r="D42" s="67"/>
       <c r="E42" s="26"/>
@@ -2563,14 +2579,8 @@
       <c r="J42" s="26"/>
       <c r="K42" s="69"/>
       <c r="L42" s="69"/>
-      <c r="M42" s="25" t="str">
-        <f t="shared" ref="M42:N42" si="31">C42+E42+G42+I42+K42</f>
-        <v>0.0</v>
-      </c>
-      <c r="N42" s="26" t="str">
-        <f t="shared" si="31"/>
-        <v>0.0</v>
-      </c>
+      <c r="M42" s="25"/>
+      <c r="N42" s="26"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
@@ -2585,30 +2595,32 @@
       <c r="Z42" s="3"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="14">
+      <c r="A43" s="29">
         <v>5.0</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="56" t="s">
         <v>44</v>
       </c>
       <c r="C43" s="67"/>
       <c r="D43" s="67"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
+      <c r="E43" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="F43" s="64">
+        <v>0.5</v>
+      </c>
       <c r="G43" s="68"/>
       <c r="H43" s="68"/>
-      <c r="I43" s="26"/>
+      <c r="I43" s="64"/>
       <c r="J43" s="26"/>
-      <c r="K43" s="69"/>
-      <c r="L43" s="69"/>
-      <c r="M43" s="25" t="str">
-        <f t="shared" ref="M43:N43" si="32">C43+E43+G43+I43+K43</f>
-        <v>0.0</v>
-      </c>
-      <c r="N43" s="26" t="str">
-        <f t="shared" si="32"/>
-        <v>0.0</v>
-      </c>
+      <c r="K43" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="L43" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="M43" s="25"/>
+      <c r="N43" s="26"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
@@ -2626,7 +2638,9 @@
       <c r="A44" s="14">
         <v>5.0</v>
       </c>
-      <c r="B44" s="79"/>
+      <c r="B44" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="C44" s="67"/>
       <c r="D44" s="67"/>
       <c r="E44" s="26"/>
@@ -2638,11 +2652,11 @@
       <c r="K44" s="69"/>
       <c r="L44" s="69"/>
       <c r="M44" s="25" t="str">
-        <f t="shared" ref="M44:N44" si="33">C44+E44+G44+I44+K44</f>
+        <f t="shared" ref="M44:N44" si="31">C44+E44+G44+I44+K44</f>
         <v>0.0</v>
       </c>
       <c r="N44" s="26" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.0</v>
       </c>
       <c r="O44" s="3"/>
@@ -2662,7 +2676,9 @@
       <c r="A45" s="14">
         <v>5.0</v>
       </c>
-      <c r="B45" s="79"/>
+      <c r="B45" s="20" t="s">
+        <v>46</v>
+      </c>
       <c r="C45" s="67"/>
       <c r="D45" s="67"/>
       <c r="E45" s="26"/>
@@ -2674,11 +2690,11 @@
       <c r="K45" s="69"/>
       <c r="L45" s="69"/>
       <c r="M45" s="25" t="str">
-        <f t="shared" ref="M45:N45" si="34">C45+E45+G45+I45+K45</f>
+        <f t="shared" ref="M45:N45" si="32">C45+E45+G45+I45+K45</f>
         <v>0.0</v>
       </c>
       <c r="N45" s="26" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="32"/>
         <v>0.0</v>
       </c>
       <c r="O45" s="3"/>
@@ -2695,20 +2711,34 @@
       <c r="Z45" s="3"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="14"/>
-      <c r="B46" s="79"/>
+      <c r="A46" s="14">
+        <v>5.0</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>35</v>
+      </c>
       <c r="C46" s="67"/>
       <c r="D46" s="67"/>
       <c r="E46" s="26"/>
       <c r="F46" s="26"/>
       <c r="G46" s="68"/>
       <c r="H46" s="68"/>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="J46" s="64">
+        <v>0.5</v>
+      </c>
       <c r="K46" s="69"/>
       <c r="L46" s="69"/>
-      <c r="M46" s="25"/>
-      <c r="N46" s="26"/>
+      <c r="M46" s="25" t="str">
+        <f t="shared" ref="M46:N46" si="33">C46+E46+G46+I46+K46</f>
+        <v>0.5</v>
+      </c>
+      <c r="N46" s="26" t="str">
+        <f t="shared" si="33"/>
+        <v>0.5</v>
+      </c>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
@@ -2724,28 +2754,44 @@
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="14">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="67"/>
-      <c r="D47" s="67"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="68"/>
-      <c r="H47" s="68"/>
+        <v>39</v>
+      </c>
+      <c r="C47" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="D47" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="E47" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="F47" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="G47" s="65">
+        <v>0.5</v>
+      </c>
+      <c r="H47" s="65">
+        <v>0.5</v>
+      </c>
       <c r="I47" s="26"/>
       <c r="J47" s="26"/>
-      <c r="K47" s="69"/>
-      <c r="L47" s="69"/>
+      <c r="K47" s="66">
+        <v>0.5</v>
+      </c>
+      <c r="L47" s="66">
+        <v>0.5</v>
+      </c>
       <c r="M47" s="25" t="str">
-        <f t="shared" ref="M47:N47" si="35">C47+E47+G47+I47+K47</f>
-        <v>0.0</v>
+        <f t="shared" ref="M47:N47" si="34">C47+E47+G47+I47+K47</f>
+        <v>2.0</v>
       </c>
       <c r="N47" s="26" t="str">
-        <f t="shared" si="35"/>
-        <v>0.0</v>
+        <f t="shared" si="34"/>
+        <v>2.0</v>
       </c>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
@@ -2762,29 +2808,21 @@
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="14">
-        <v>6.0</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" s="80"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="81"/>
-      <c r="H48" s="81"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
+        <v>5.0</v>
+      </c>
+      <c r="B48" s="79"/>
+      <c r="C48" s="67"/>
+      <c r="D48" s="67"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="68"/>
+      <c r="H48" s="68"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
       <c r="K48" s="69"/>
       <c r="L48" s="69"/>
-      <c r="M48" s="25" t="str">
-        <f t="shared" ref="M48:N48" si="36">C48+E48+G48+I48+K48</f>
-        <v>0.0</v>
-      </c>
-      <c r="N48" s="26" t="str">
-        <f t="shared" si="36"/>
-        <v>0.0</v>
-      </c>
+      <c r="M48" s="25"/>
+      <c r="N48" s="26"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
@@ -2802,23 +2840,25 @@
       <c r="A49" s="14">
         <v>6.0</v>
       </c>
-      <c r="B49" s="79"/>
-      <c r="C49" s="80"/>
-      <c r="D49" s="80"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="81"/>
-      <c r="H49" s="81"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
+      <c r="B49" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="67"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="68"/>
+      <c r="H49" s="68"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
       <c r="K49" s="69"/>
       <c r="L49" s="69"/>
       <c r="M49" s="25" t="str">
-        <f t="shared" ref="M49:N49" si="37">C49+E49+G49+I49+K49</f>
+        <f t="shared" ref="M49:N49" si="35">C49+E49+G49+I49+K49</f>
         <v>0.0</v>
       </c>
       <c r="N49" s="26" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="35"/>
         <v>0.0</v>
       </c>
       <c r="O49" s="3"/>
@@ -2838,7 +2878,9 @@
       <c r="A50" s="14">
         <v>6.0</v>
       </c>
-      <c r="B50" s="79"/>
+      <c r="B50" s="20" t="s">
+        <v>45</v>
+      </c>
       <c r="C50" s="80"/>
       <c r="D50" s="80"/>
       <c r="E50" s="14"/>
@@ -2850,11 +2892,11 @@
       <c r="K50" s="69"/>
       <c r="L50" s="69"/>
       <c r="M50" s="25" t="str">
-        <f t="shared" ref="M50:N50" si="38">C50+E50+G50+I50+K50</f>
+        <f t="shared" ref="M50:N50" si="36">C50+E50+G50+I50+K50</f>
         <v>0.0</v>
       </c>
       <c r="N50" s="26" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>0.0</v>
       </c>
       <c r="O50" s="3"/>
@@ -2886,11 +2928,11 @@
       <c r="K51" s="69"/>
       <c r="L51" s="69"/>
       <c r="M51" s="25" t="str">
-        <f t="shared" ref="M51:N51" si="39">C51+E51+G51+I51+K51</f>
+        <f t="shared" ref="M51:N51" si="37">C51+E51+G51+I51+K51</f>
         <v>0.0</v>
       </c>
       <c r="N51" s="26" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>0.0</v>
       </c>
       <c r="O51" s="3"/>
@@ -2922,17 +2964,30 @@
       <c r="K52" s="69"/>
       <c r="L52" s="69"/>
       <c r="M52" s="25" t="str">
-        <f t="shared" ref="M52:N52" si="40">C52+E52+G52+I52+K52</f>
+        <f t="shared" ref="M52:N52" si="38">C52+E52+G52+I52+K52</f>
         <v>0.0</v>
       </c>
       <c r="N52" s="26" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>0.0</v>
       </c>
       <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+      <c r="V52" s="3"/>
+      <c r="W52" s="3"/>
+      <c r="X52" s="3"/>
+      <c r="Y52" s="3"/>
+      <c r="Z52" s="3"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="14"/>
+      <c r="A53" s="14">
+        <v>6.0</v>
+      </c>
       <c r="B53" s="79"/>
       <c r="C53" s="80"/>
       <c r="D53" s="80"/>
@@ -2944,18 +2999,33 @@
       <c r="J53" s="14"/>
       <c r="K53" s="69"/>
       <c r="L53" s="69"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="26"/>
+      <c r="M53" s="25" t="str">
+        <f t="shared" ref="M53:N53" si="39">C53+E53+G53+I53+K53</f>
+        <v>0.0</v>
+      </c>
+      <c r="N53" s="26" t="str">
+        <f t="shared" si="39"/>
+        <v>0.0</v>
+      </c>
       <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="3"/>
+      <c r="U53" s="3"/>
+      <c r="V53" s="3"/>
+      <c r="W53" s="3"/>
+      <c r="X53" s="3"/>
+      <c r="Y53" s="3"/>
+      <c r="Z53" s="3"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B54" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C54" s="82"/>
+      <c r="A54" s="14">
+        <v>6.0</v>
+      </c>
+      <c r="B54" s="79"/>
+      <c r="C54" s="80"/>
       <c r="D54" s="80"/>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
@@ -2966,22 +3036,18 @@
       <c r="K54" s="69"/>
       <c r="L54" s="69"/>
       <c r="M54" s="25" t="str">
-        <f t="shared" ref="M54:N54" si="41">C54+E54+G54+I54+K54</f>
+        <f t="shared" ref="M54:N54" si="40">C54+E54+G54+I54+K54</f>
         <v>0.0</v>
       </c>
       <c r="N54" s="26" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>0.0</v>
       </c>
       <c r="O54" s="3"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" s="20" t="s">
-        <v>47</v>
-      </c>
+      <c r="A55" s="14"/>
+      <c r="B55" s="79"/>
       <c r="C55" s="80"/>
       <c r="D55" s="80"/>
       <c r="E55" s="14"/>
@@ -2992,23 +3058,18 @@
       <c r="J55" s="14"/>
       <c r="K55" s="69"/>
       <c r="L55" s="69"/>
-      <c r="M55" s="25" t="str">
-        <f t="shared" ref="M55:N55" si="42">C55+E55+G55+I55+K55</f>
-        <v>0.0</v>
-      </c>
-      <c r="N55" s="26" t="str">
-        <f t="shared" si="42"/>
-        <v>0.0</v>
-      </c>
+      <c r="M55" s="25"/>
+      <c r="N55" s="26"/>
+      <c r="O55" s="3"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
       <c r="A56" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B56" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="80"/>
+      <c r="C56" s="82"/>
       <c r="D56" s="80"/>
       <c r="E56" s="14"/>
       <c r="F56" s="14"/>
@@ -3019,17 +3080,18 @@
       <c r="K56" s="69"/>
       <c r="L56" s="69"/>
       <c r="M56" s="25" t="str">
-        <f t="shared" ref="M56:N56" si="43">C56+E56+G56+I56+K56</f>
+        <f t="shared" ref="M56:N56" si="41">C56+E56+G56+I56+K56</f>
         <v>0.0</v>
       </c>
       <c r="N56" s="26" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="41"/>
         <v>0.0</v>
       </c>
+      <c r="O56" s="3"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
       <c r="A57" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B57" s="20" t="s">
         <v>49</v>
@@ -3045,17 +3107,17 @@
       <c r="K57" s="69"/>
       <c r="L57" s="69"/>
       <c r="M57" s="25" t="str">
-        <f t="shared" ref="M57:N57" si="44">C57+E57+G57+I57+K57</f>
+        <f t="shared" ref="M57:N57" si="42">C57+E57+G57+I57+K57</f>
         <v>0.0</v>
       </c>
       <c r="N57" s="26" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="42"/>
         <v>0.0</v>
       </c>
     </row>
     <row r="58" ht="12.75" customHeight="1">
       <c r="A58" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>50</v>
@@ -3071,19 +3133,21 @@
       <c r="K58" s="69"/>
       <c r="L58" s="69"/>
       <c r="M58" s="25" t="str">
-        <f t="shared" ref="M58:N58" si="45">C58+E58+G58+I58+K58</f>
+        <f t="shared" ref="M58:N58" si="43">C58+E58+G58+I58+K58</f>
         <v>0.0</v>
       </c>
       <c r="N58" s="26" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="43"/>
         <v>0.0</v>
       </c>
     </row>
     <row r="59" ht="12.75" customHeight="1">
       <c r="A59" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B59" s="79"/>
+        <v>47</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>51</v>
+      </c>
       <c r="C59" s="80"/>
       <c r="D59" s="80"/>
       <c r="E59" s="14"/>
@@ -3095,17 +3159,21 @@
       <c r="K59" s="69"/>
       <c r="L59" s="69"/>
       <c r="M59" s="25" t="str">
-        <f t="shared" ref="M59:N59" si="46">C59+E59+G59+I59+K59</f>
+        <f t="shared" ref="M59:N59" si="44">C59+E59+G59+I59+K59</f>
         <v>0.0</v>
       </c>
       <c r="N59" s="26" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="44"/>
         <v>0.0</v>
       </c>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="14"/>
-      <c r="B60" s="79"/>
+      <c r="A60" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>52</v>
+      </c>
       <c r="C60" s="80"/>
       <c r="D60" s="80"/>
       <c r="E60" s="14"/>
@@ -3116,168 +3184,166 @@
       <c r="J60" s="14"/>
       <c r="K60" s="69"/>
       <c r="L60" s="69"/>
-      <c r="M60" s="25"/>
-      <c r="N60" s="26"/>
+      <c r="M60" s="25" t="str">
+        <f t="shared" ref="M60:N60" si="45">C60+E60+G60+I60+K60</f>
+        <v>0.0</v>
+      </c>
+      <c r="N60" s="26" t="str">
+        <f t="shared" si="45"/>
+        <v>0.0</v>
+      </c>
     </row>
     <row r="61" ht="12.75" customHeight="1">
       <c r="A61" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B61" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C61" s="82">
-        <v>2.0</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B61" s="79"/>
+      <c r="C61" s="80"/>
       <c r="D61" s="80"/>
-      <c r="E61" s="29">
-        <v>2.0</v>
-      </c>
+      <c r="E61" s="14"/>
       <c r="F61" s="14"/>
-      <c r="G61" s="83">
-        <v>2.0</v>
-      </c>
+      <c r="G61" s="81"/>
       <c r="H61" s="81"/>
-      <c r="I61" s="29">
-        <v>2.0</v>
-      </c>
+      <c r="I61" s="14"/>
       <c r="J61" s="14"/>
-      <c r="K61" s="66">
-        <v>2.0</v>
-      </c>
+      <c r="K61" s="69"/>
       <c r="L61" s="69"/>
       <c r="M61" s="25" t="str">
-        <f t="shared" ref="M61:N61" si="47">C61+E61+G61+I61+K61</f>
+        <f t="shared" ref="M61:N61" si="46">C61+E61+G61+I61+K61</f>
+        <v>0.0</v>
+      </c>
+      <c r="N61" s="26" t="str">
+        <f t="shared" si="46"/>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="62" ht="12.75" customHeight="1">
+      <c r="A62" s="14"/>
+      <c r="B62" s="79"/>
+      <c r="C62" s="80"/>
+      <c r="D62" s="80"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="81"/>
+      <c r="H62" s="81"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="69"/>
+      <c r="L62" s="69"/>
+      <c r="M62" s="25"/>
+      <c r="N62" s="26"/>
+    </row>
+    <row r="63" ht="12.75" customHeight="1">
+      <c r="A63" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C63" s="82">
+        <v>2.0</v>
+      </c>
+      <c r="D63" s="80"/>
+      <c r="E63" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="F63" s="14"/>
+      <c r="G63" s="83">
+        <v>2.0</v>
+      </c>
+      <c r="H63" s="81"/>
+      <c r="I63" s="29">
+        <v>2.0</v>
+      </c>
+      <c r="J63" s="14"/>
+      <c r="K63" s="66">
+        <v>2.0</v>
+      </c>
+      <c r="L63" s="69"/>
+      <c r="M63" s="25" t="str">
+        <f t="shared" ref="M63:N63" si="47">C63+E63+G63+I63+K63</f>
         <v>10.0</v>
       </c>
-      <c r="N61" s="26" t="str">
+      <c r="N63" s="26" t="str">
         <f t="shared" si="47"/>
         <v>0.0</v>
       </c>
     </row>
-    <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B62" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C62" s="82">
+    <row r="64" ht="12.75" customHeight="1">
+      <c r="A64" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" s="82">
         <v>5.0</v>
       </c>
-      <c r="D62" s="80"/>
-      <c r="E62" s="29">
+      <c r="D64" s="80"/>
+      <c r="E64" s="29">
         <v>5.0</v>
       </c>
-      <c r="F62" s="14"/>
-      <c r="G62" s="83">
+      <c r="F64" s="14"/>
+      <c r="G64" s="83">
         <v>5.0</v>
       </c>
-      <c r="H62" s="81"/>
-      <c r="I62" s="29">
+      <c r="H64" s="81"/>
+      <c r="I64" s="29">
         <v>5.0</v>
       </c>
-      <c r="J62" s="14"/>
-      <c r="K62" s="66">
+      <c r="J64" s="14"/>
+      <c r="K64" s="66">
         <v>5.0</v>
       </c>
-      <c r="L62" s="69"/>
-      <c r="M62" s="25" t="str">
-        <f t="shared" ref="M62:N62" si="48">C62+E62+G62+I62+K62</f>
+      <c r="L64" s="69"/>
+      <c r="M64" s="25" t="str">
+        <f t="shared" ref="M64:N64" si="48">C64+E64+G64+I64+K64</f>
         <v>25.0</v>
       </c>
-      <c r="N62" s="26" t="str">
+      <c r="N64" s="26" t="str">
         <f t="shared" si="48"/>
         <v>0.0</v>
       </c>
     </row>
-    <row r="63" ht="12.75" customHeight="1">
-      <c r="A63" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B63" s="20" t="s">
+    <row r="65" ht="12.75" customHeight="1">
+      <c r="A65" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C63" s="82">
+      <c r="B65" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C65" s="82">
         <v>5.0</v>
       </c>
-      <c r="D63" s="82"/>
-      <c r="E63" s="29">
+      <c r="D65" s="82"/>
+      <c r="E65" s="29">
         <v>5.0</v>
       </c>
-      <c r="F63" s="29"/>
-      <c r="G63" s="83">
+      <c r="F65" s="29"/>
+      <c r="G65" s="83">
         <v>5.0</v>
       </c>
-      <c r="H63" s="81"/>
-      <c r="I63" s="29">
+      <c r="H65" s="81"/>
+      <c r="I65" s="29">
         <v>5.0</v>
       </c>
-      <c r="J63" s="14"/>
-      <c r="K63" s="66">
+      <c r="J65" s="14"/>
+      <c r="K65" s="66">
         <v>5.0</v>
       </c>
-      <c r="L63" s="69"/>
-      <c r="M63" s="25" t="str">
-        <f t="shared" ref="M63:N63" si="49">C63+E63+G63+I63+K63</f>
+      <c r="L65" s="69"/>
+      <c r="M65" s="25" t="str">
+        <f t="shared" ref="M65:N65" si="49">C65+E65+G65+I65+K65</f>
         <v>25.0</v>
       </c>
-      <c r="N63" s="26" t="str">
+      <c r="N65" s="26" t="str">
         <f t="shared" si="49"/>
         <v>0.0</v>
       </c>
     </row>
-    <row r="64" ht="13.5" customHeight="1">
-      <c r="A64" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B64" s="79"/>
-      <c r="C64" s="80"/>
-      <c r="D64" s="80"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="81"/>
-      <c r="H64" s="81"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="69"/>
-      <c r="L64" s="69"/>
-      <c r="M64" s="25" t="str">
-        <f t="shared" ref="M64:N64" si="50">C64+E64+G64+I64+K64</f>
-        <v>0.0</v>
-      </c>
-      <c r="N64" s="26" t="str">
-        <f t="shared" si="50"/>
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="65" ht="12.75" customHeight="1">
-      <c r="A65" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B65" s="79"/>
-      <c r="C65" s="80"/>
-      <c r="D65" s="80"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="81"/>
-      <c r="H65" s="81"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="69"/>
-      <c r="L65" s="69"/>
-      <c r="M65" s="25" t="str">
-        <f t="shared" ref="M65:N65" si="51">C65+E65+G65+I65+K65</f>
-        <v>0.0</v>
-      </c>
-      <c r="N65" s="26" t="str">
-        <f t="shared" si="51"/>
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="66" ht="12.75" customHeight="1">
+    <row r="66" ht="13.5" customHeight="1">
       <c r="A66" s="14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B66" s="79"/>
       <c r="C66" s="80"/>
@@ -3291,119 +3357,135 @@
       <c r="K66" s="69"/>
       <c r="L66" s="69"/>
       <c r="M66" s="25" t="str">
-        <f t="shared" ref="M66:N66" si="52">C66+E66+G66+I66+K66</f>
+        <f t="shared" ref="M66:N66" si="50">C66+E66+G66+I66+K66</f>
         <v>0.0</v>
       </c>
       <c r="N66" s="26" t="str">
+        <f t="shared" si="50"/>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="67" ht="12.75" customHeight="1">
+      <c r="A67" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" s="79"/>
+      <c r="C67" s="80"/>
+      <c r="D67" s="80"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="81"/>
+      <c r="H67" s="81"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="69"/>
+      <c r="L67" s="69"/>
+      <c r="M67" s="25" t="str">
+        <f t="shared" ref="M67:N67" si="51">C67+E67+G67+I67+K67</f>
+        <v>0.0</v>
+      </c>
+      <c r="N67" s="26" t="str">
+        <f t="shared" si="51"/>
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="68" ht="12.75" customHeight="1">
+      <c r="A68" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B68" s="79"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="80"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="81"/>
+      <c r="H68" s="81"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="69"/>
+      <c r="L68" s="69"/>
+      <c r="M68" s="25" t="str">
+        <f t="shared" ref="M68:N68" si="52">C68+E68+G68+I68+K68</f>
+        <v>0.0</v>
+      </c>
+      <c r="N68" s="26" t="str">
         <f t="shared" si="52"/>
         <v>0.0</v>
       </c>
     </row>
-    <row r="67" ht="12.75" customHeight="1">
-      <c r="A67" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B67" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="C67" s="84"/>
-      <c r="D67" s="84"/>
-      <c r="E67" s="79"/>
-      <c r="F67" s="79"/>
-      <c r="G67" s="85"/>
-      <c r="H67" s="85"/>
-      <c r="I67" s="79"/>
-      <c r="J67" s="79"/>
-      <c r="K67" s="69"/>
-      <c r="L67" s="69"/>
-      <c r="M67" s="86"/>
-      <c r="N67" s="87"/>
-    </row>
-    <row r="68" ht="12.75" customHeight="1">
-      <c r="A68" s="88"/>
-      <c r="B68" s="89" t="s">
+    <row r="69" ht="12.75" customHeight="1">
+      <c r="A69" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C68" s="90" t="str">
-        <f t="shared" ref="C68:L68" si="53">SUM(C5:C63)</f>
-        <v>34.5</v>
-      </c>
-      <c r="D68" s="90" t="str">
+      <c r="B69" s="77" t="s">
+        <v>57</v>
+      </c>
+      <c r="C69" s="84"/>
+      <c r="D69" s="84"/>
+      <c r="E69" s="79"/>
+      <c r="F69" s="79"/>
+      <c r="G69" s="85"/>
+      <c r="H69" s="85"/>
+      <c r="I69" s="79"/>
+      <c r="J69" s="79"/>
+      <c r="K69" s="69"/>
+      <c r="L69" s="69"/>
+      <c r="M69" s="86"/>
+      <c r="N69" s="87"/>
+    </row>
+    <row r="70" ht="12.75" customHeight="1">
+      <c r="A70" s="88"/>
+      <c r="B70" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" s="90" t="str">
+        <f t="shared" ref="C70:L70" si="53">SUM(C5:C65)</f>
+        <v>35.0</v>
+      </c>
+      <c r="D70" s="90" t="str">
         <f t="shared" si="53"/>
-        <v>19.7</v>
-      </c>
-      <c r="E68" s="90" t="str">
+        <v>20.2</v>
+      </c>
+      <c r="E70" s="90" t="str">
         <f t="shared" si="53"/>
-        <v>30.3</v>
-      </c>
-      <c r="F68" s="90" t="str">
+        <v>31.3</v>
+      </c>
+      <c r="F70" s="90" t="str">
         <f t="shared" si="53"/>
-        <v>16.3</v>
-      </c>
-      <c r="G68" s="90" t="str">
-        <f t="shared" si="53"/>
-        <v>33.0</v>
-      </c>
-      <c r="H68" s="90" t="str">
-        <f t="shared" si="53"/>
-        <v>17.5</v>
-      </c>
-      <c r="I68" s="90" t="str">
+        <v>19.3</v>
+      </c>
+      <c r="G70" s="90" t="str">
         <f t="shared" si="53"/>
         <v>33.5</v>
       </c>
-      <c r="J68" s="90" t="str">
+      <c r="H70" s="90" t="str">
         <f t="shared" si="53"/>
-        <v>17.5</v>
-      </c>
-      <c r="K68" s="90" t="str">
+        <v>22.0</v>
+      </c>
+      <c r="I70" s="90" t="str">
         <f t="shared" si="53"/>
-        <v>31.1</v>
-      </c>
-      <c r="L68" s="90" t="str">
+        <v>34.0</v>
+      </c>
+      <c r="J70" s="90" t="str">
         <f t="shared" si="53"/>
-        <v>17.6</v>
-      </c>
-      <c r="M68" s="90" t="str">
-        <f t="shared" ref="M68:N68" si="54">C68+E68+G68+I68+K68</f>
-        <v>162.4</v>
-      </c>
-      <c r="N68" s="90" t="str">
+        <v>18.0</v>
+      </c>
+      <c r="K70" s="90" t="str">
+        <f t="shared" si="53"/>
+        <v>32.1</v>
+      </c>
+      <c r="L70" s="90" t="str">
+        <f t="shared" si="53"/>
+        <v>20.6</v>
+      </c>
+      <c r="M70" s="90" t="str">
+        <f t="shared" ref="M70:N70" si="54">C70+E70+G70+I70+K70</f>
+        <v>165.9</v>
+      </c>
+      <c r="N70" s="90" t="str">
         <f t="shared" si="54"/>
-        <v>88.6</v>
-      </c>
-    </row>
-    <row r="69" ht="12.75" customHeight="1">
-      <c r="A69" s="91"/>
-      <c r="B69" s="91"/>
-      <c r="C69" s="91"/>
-      <c r="D69" s="91"/>
-      <c r="E69" s="91"/>
-      <c r="F69" s="91"/>
-      <c r="G69" s="91"/>
-      <c r="H69" s="91"/>
-      <c r="I69" s="91"/>
-      <c r="J69" s="91"/>
-      <c r="K69" s="91"/>
-      <c r="L69" s="91"/>
-      <c r="M69" s="91"/>
-      <c r="N69" s="91"/>
-    </row>
-    <row r="70" ht="12.75" customHeight="1">
-      <c r="A70" s="91"/>
-      <c r="B70" s="91"/>
-      <c r="C70" s="91"/>
-      <c r="D70" s="91"/>
-      <c r="E70" s="91"/>
-      <c r="F70" s="91"/>
-      <c r="G70" s="91"/>
-      <c r="H70" s="91"/>
-      <c r="I70" s="91"/>
-      <c r="J70" s="91"/>
-      <c r="K70" s="91"/>
-      <c r="L70" s="91"/>
-      <c r="M70" s="91"/>
-      <c r="N70" s="91"/>
+        <v>100.1</v>
+      </c>
     </row>
     <row r="71" ht="12.75" customHeight="1">
       <c r="A71" s="91"/>
@@ -18604,6 +18686,38 @@
       <c r="L1020" s="91"/>
       <c r="M1020" s="91"/>
       <c r="N1020" s="91"/>
+    </row>
+    <row r="1021" ht="12.75" customHeight="1">
+      <c r="A1021" s="91"/>
+      <c r="B1021" s="91"/>
+      <c r="C1021" s="91"/>
+      <c r="D1021" s="91"/>
+      <c r="E1021" s="91"/>
+      <c r="F1021" s="91"/>
+      <c r="G1021" s="91"/>
+      <c r="H1021" s="91"/>
+      <c r="I1021" s="91"/>
+      <c r="J1021" s="91"/>
+      <c r="K1021" s="91"/>
+      <c r="L1021" s="91"/>
+      <c r="M1021" s="91"/>
+      <c r="N1021" s="91"/>
+    </row>
+    <row r="1022" ht="12.75" customHeight="1">
+      <c r="A1022" s="91"/>
+      <c r="B1022" s="91"/>
+      <c r="C1022" s="91"/>
+      <c r="D1022" s="91"/>
+      <c r="E1022" s="91"/>
+      <c r="F1022" s="91"/>
+      <c r="G1022" s="91"/>
+      <c r="H1022" s="91"/>
+      <c r="I1022" s="91"/>
+      <c r="J1022" s="91"/>
+      <c r="K1022" s="91"/>
+      <c r="L1022" s="91"/>
+      <c r="M1022" s="91"/>
+      <c r="N1022" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>